<commit_message>
make the DFs refresh after every updating
</commit_message>
<xml_diff>
--- a/sample_main.xlsx
+++ b/sample_main.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\acer\Documents\GitHub\HomeStocks\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E4EAC7-6A88-452E-BF31-60DFAB99EADC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="276" yWindow="564" windowWidth="21852" windowHeight="11916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
   <si>
     <t>区域</t>
   </si>
@@ -37,101 +31,104 @@
     <t>基地洗手间</t>
   </si>
   <si>
+    <t>基地厨房</t>
+  </si>
+  <si>
+    <t>测试区域</t>
+  </si>
+  <si>
+    <t>天上</t>
+  </si>
+  <si>
+    <t>我的世界</t>
+  </si>
+  <si>
     <t>书柜1</t>
   </si>
   <si>
+    <t>银色架子</t>
+  </si>
+  <si>
     <t>书柜2</t>
   </si>
   <si>
-    <t>银色架子</t>
+    <t>白柜子1</t>
+  </si>
+  <si>
+    <t>白柜子2</t>
+  </si>
+  <si>
+    <t>西门子</t>
   </si>
   <si>
     <t>测试词</t>
   </si>
   <si>
-    <t>天上</t>
-  </si>
-  <si>
     <t>白云</t>
   </si>
   <si>
-    <t>我的世界</t>
-  </si>
-  <si>
     <t>下界</t>
   </si>
   <si>
+    <t>口罩、绿茶茶叶、红茶茶叶、咖啡杯</t>
+  </si>
+  <si>
+    <t>红茶茶叶、咖啡壶</t>
+  </si>
+  <si>
+    <t>面膜、红茶茶叶、学历、袜子、泳镜、茉莉花、奶粉罐、锅勺</t>
+  </si>
+  <si>
+    <t>遥控器、红茶茶叶、遥控器、遥控器、遥控器、遥控器</t>
+  </si>
+  <si>
+    <t>燕麦、奇亚籽、藜麦、豆浆粉、面粉、可可粉、咖啡研磨器</t>
+  </si>
+  <si>
+    <t>一次性餐具、纸杯、搅拌机、料理机、厨师机</t>
+  </si>
+  <si>
+    <t>蛋糕模具、菜刀、荞麦面刀、切冰刀</t>
+  </si>
+  <si>
+    <t>西红柿罐头、鹰嘴豆罐头、吞拿鱼罐头、玉米罐头、芦笋罐头、腌黄瓜</t>
+  </si>
+  <si>
+    <t>牛排、照烧酱、牛奶、杏仁奶、燕麦奶</t>
+  </si>
+  <si>
+    <t>玫瑰葡萄酒、玫瑰汽水、生菜、西葫芦、巴沙鱼、三文鱼</t>
+  </si>
+  <si>
+    <t>生姜、巧克力、樱桃、香蕉、梨子</t>
+  </si>
+  <si>
+    <t>眼膜、鸡蛋、三明治、关东煮、布鲁塞尔豆芽</t>
+  </si>
+  <si>
+    <t>西兰花、什锦蔬菜、竹轮卷、鸣门卷、羊肉片</t>
+  </si>
+  <si>
+    <t>香烟、啤酒、可乐、西红柿</t>
+  </si>
+  <si>
+    <t>咖喱棒、狮子玩偶、红宝石吊坠、章鱼烧</t>
+  </si>
+  <si>
+    <t>红刷子、黄刷子、世界地图、钢琴</t>
+  </si>
+  <si>
+    <t>沙漏</t>
+  </si>
+  <si>
     <t>黑曜石</t>
-  </si>
-  <si>
-    <t>沙漏</t>
-  </si>
-  <si>
-    <t>咖喱棒、狮子玩偶、红宝石吊坠、章鱼烧</t>
-  </si>
-  <si>
-    <t>红刷子、黄刷子、世界地图、钢琴</t>
-  </si>
-  <si>
-    <t>西门子</t>
-  </si>
-  <si>
-    <t>白柜子1</t>
-  </si>
-  <si>
-    <t>白柜子2</t>
-  </si>
-  <si>
-    <t>生姜、巧克力、樱桃、香蕉、梨子</t>
-  </si>
-  <si>
-    <t>香烟、啤酒、可乐、西红柿</t>
-  </si>
-  <si>
-    <t>牛排、照烧酱、牛奶、杏仁奶、燕麦奶</t>
-  </si>
-  <si>
-    <t>眼膜、鸡蛋、三明治、关东煮、布鲁塞尔豆芽</t>
-  </si>
-  <si>
-    <t>西兰花、什锦蔬菜、竹轮卷、鸣门卷、羊肉片</t>
-  </si>
-  <si>
-    <t>一次性餐具、纸杯、搅拌机、料理机、厨师机</t>
-  </si>
-  <si>
-    <t>蛋糕模具、菜刀、荞麦面刀、切冰刀</t>
-  </si>
-  <si>
-    <t>西红柿罐头、鹰嘴豆罐头、吞拿鱼罐头、玉米罐头、芦笋罐头、腌黄瓜</t>
-  </si>
-  <si>
-    <t>基地厨房</t>
-  </si>
-  <si>
-    <t>玫瑰葡萄酒、玫瑰汽水、生菜、西葫芦、巴沙鱼、三文鱼</t>
-  </si>
-  <si>
-    <t>面膜、红茶茶叶、学历、袜子、泳镜、茉莉花、奶粉罐、锅勺</t>
-  </si>
-  <si>
-    <t>口罩、绿茶茶叶、红茶茶叶、咖啡杯</t>
-  </si>
-  <si>
-    <t>红茶茶叶、咖啡壶</t>
-  </si>
-  <si>
-    <t>燕麦、奇亚籽、藜麦、豆浆粉、面粉、可可粉、咖啡研磨器</t>
-  </si>
-  <si>
-    <t>遥控器、红茶茶叶、遥控器、遥控器、遥控器、遥控器</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,12 +140,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -189,13 +180,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -203,14 +191,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -257,7 +237,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -289,27 +269,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,24 +303,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -534,20 +478,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,174 +496,205 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>